<commit_message>
aufgabe 3 besser, 5 angefangen
</commit_message>
<xml_diff>
--- a/RN_UE11_3.xlsx
+++ b/RN_UE11_3.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenboda/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Apps\OMNET\workspace\git\RN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="460" windowWidth="15460" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="6945" yWindow="465" windowWidth="15465" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,103 +27,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="20">
   <si>
     <t>von Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>∞</t>
   </si>
   <si>
     <t>∞</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zu v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zu z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zu u</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>via x</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>via v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>via z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>via u</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zu y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>via y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zu x</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>von X</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>von V</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>von Z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>von U</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>V:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>X:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Z:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="DengXian"/>
       <family val="2"/>
       <charset val="134"/>
@@ -167,6 +159,19 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -214,33 +219,37 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -511,13 +520,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="125" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,26 +548,26 @@
       <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -577,26 +586,26 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -615,26 +624,26 @@
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="5">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>8</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -653,26 +662,26 @@
       <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -691,26 +700,26 @@
       <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -729,11 +738,11 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="2">
-        <v>8</v>
+      <c r="I6" s="8">
+        <v>5</v>
       </c>
       <c r="J6" s="6">
         <v>3</v>
@@ -741,14 +750,30 @@
       <c r="K6" s="6">
         <v>7</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="M6" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -770,26 +795,26 @@
       <c r="G9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="H9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="L9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -808,26 +833,26 @@
       <c r="F10" s="1">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>2</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="L10" s="5">
-        <v>17</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="M10" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -846,26 +871,26 @@
       <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="5">
         <v>5</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="J11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="5">
         <v>8</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -884,26 +909,26 @@
       <c r="F12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -922,26 +947,26 @@
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -960,11 +985,11 @@
       <c r="F14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="2">
-        <v>8</v>
+      <c r="I14" s="6">
+        <v>5</v>
       </c>
       <c r="J14" s="6">
         <v>3</v>
@@ -972,14 +997,30 @@
       <c r="K14" s="6">
         <v>7</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>2</v>
+      <c r="L14" s="8">
+        <v>17</v>
       </c>
       <c r="M14" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1001,26 +1042,26 @@
       <c r="G17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="H17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M17" s="3" t="s">
+      <c r="L17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1039,26 +1080,26 @@
       <c r="F18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="7">
-        <v>17</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>2</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="5">
+        <v>12</v>
+      </c>
+      <c r="M18" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1077,26 +1118,26 @@
       <c r="F19" s="1">
         <v>3</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I19" s="5">
         <v>5</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" s="1">
+      <c r="J19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5">
         <v>8</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1115,26 +1156,26 @@
       <c r="F20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>1</v>
+      <c r="I20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5">
+        <v>5</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
       </c>
       <c r="L20" s="5">
-        <v>11</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="M20" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1153,26 +1194,26 @@
       <c r="F21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1191,11 +1232,11 @@
       <c r="F22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="2">
-        <v>8</v>
+      <c r="I22" s="6">
+        <v>5</v>
       </c>
       <c r="J22" s="6">
         <v>3</v>
@@ -1203,14 +1244,14 @@
       <c r="K22" s="6">
         <v>7</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>2</v>
+      <c r="L22" s="8">
+        <v>11</v>
       </c>
       <c r="M22" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1230,7 +1271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1250,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1310,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -1330,7 +1371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +1391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1390,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
@@ -1410,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1430,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>11</v>
       </c>
@@ -1451,7 +1492,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aufgabe 3 noch besser
</commit_message>
<xml_diff>
--- a/RN_UE11_3.xlsx
+++ b/RN_UE11_3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="20">
   <si>
     <t>von Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,30 +52,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>via x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>via v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>via z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>via u</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>zu y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>via y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>zu x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,6 +86,21 @@
   <si>
     <t>Z:</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>von x</t>
+  </si>
+  <si>
+    <t>von v</t>
+  </si>
+  <si>
+    <t>von z</t>
+  </si>
+  <si>
+    <t>von u</t>
+  </si>
+  <si>
+    <t>von y</t>
   </si>
 </sst>
 </file>
@@ -224,7 +219,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -234,6 +229,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -521,7 +517,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -531,7 +527,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -543,16 +539,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>3</v>
@@ -564,12 +560,12 @@
         <v>5</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -587,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>1</v>
@@ -607,7 +603,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -625,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I3" s="5">
         <v>2</v>
@@ -645,7 +641,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -663,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>1</v>
@@ -683,7 +679,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -701,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>2</v>
@@ -721,7 +717,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>8</v>
@@ -739,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I6" s="8">
         <v>5</v>
@@ -775,10 +771,10 @@
     </row>
     <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>3</v>
@@ -790,16 +786,16 @@
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>3</v>
@@ -811,12 +807,12 @@
         <v>5</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -834,7 +830,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I10" s="5">
         <v>0</v>
@@ -854,7 +850,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -872,27 +868,27 @@
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I11" s="5">
-        <v>5</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
       </c>
       <c r="K11" s="5">
-        <v>8</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="L11" s="9">
+        <v>14</v>
+      </c>
+      <c r="M11" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -910,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>1</v>
@@ -930,7 +926,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
@@ -948,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>2</v>
@@ -968,7 +964,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
@@ -986,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I14" s="6">
         <v>5</v>
@@ -1022,10 +1018,10 @@
     </row>
     <row r="17" spans="1:13" ht="15.75">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>3</v>
@@ -1037,16 +1033,16 @@
         <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>3</v>
@@ -1058,12 +1054,12 @@
         <v>5</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
@@ -1081,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I18" s="5">
         <v>0</v>
@@ -1089,19 +1085,19 @@
       <c r="J18" s="5">
         <v>2</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="5">
-        <v>12</v>
-      </c>
-      <c r="M18" s="5">
-        <v>8</v>
+      <c r="K18" s="9">
+        <v>7</v>
+      </c>
+      <c r="L18" s="9">
+        <v>11</v>
+      </c>
+      <c r="M18" s="9">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -1119,27 +1115,27 @@
         <v>3</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I19" s="5">
-        <v>5</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
       </c>
       <c r="K19" s="5">
-        <v>8</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="L19" s="9">
+        <v>9</v>
+      </c>
+      <c r="M19" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -1157,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>1</v>
@@ -1177,7 +1173,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>2</v>
@@ -1195,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>2</v>
@@ -1215,7 +1211,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
@@ -1233,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I22" s="6">
         <v>5</v>
@@ -1253,10 +1249,10 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>3</v>
@@ -1268,12 +1264,12 @@
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>1</v>
@@ -1293,7 +1289,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1</v>
@@ -1313,7 +1309,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
@@ -1333,7 +1329,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>2</v>
@@ -1353,7 +1349,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>2</v>
@@ -1373,10 +1369,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>3</v>
@@ -1388,12 +1384,12 @@
         <v>5</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
@@ -1413,7 +1409,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>
@@ -1433,7 +1429,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>1</v>
@@ -1453,7 +1449,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B37" s="1">
         <v>12</v>
@@ -1473,7 +1469,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>2</v>
@@ -1494,5 +1490,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>